<commit_message>
New Classes &  Objects
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\EJAR_UAT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70B2CF9-F342-4CB4-BC8A-2A61E7463E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D529DC3-E032-4515-B060-72C9D227BC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuiteDetails" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="273">
   <si>
     <t>P_Key</t>
   </si>
@@ -255,12 +255,6 @@
     <t>BO_AutomationTest12</t>
   </si>
   <si>
-    <t>1098789098</t>
-  </si>
-  <si>
-    <t>1000211100</t>
-  </si>
-  <si>
     <t>Add new Commercial contract</t>
   </si>
   <si>
@@ -450,9 +444,6 @@
     <t>20157310670</t>
   </si>
   <si>
-    <t>ApproveContractTenant2</t>
-  </si>
-  <si>
     <t>Verify Bo Officer Able To Create Account After Admin Approval</t>
   </si>
   <si>
@@ -480,24 +471,15 @@
     <t>TC05_VerifyBoOfficerAbleToCheckRegistrationApprovedStatus</t>
   </si>
   <si>
-    <t>ResidentialContract2</t>
-  </si>
-  <si>
     <t>AddResidentialContract~ApproveContractLesser2</t>
   </si>
   <si>
-    <t>ApproveContractLesser2</t>
-  </si>
-  <si>
     <t>AddResidentialContract~ResidentialContract2</t>
   </si>
   <si>
     <t>AddResidentialContract~ApproveContractTenant2</t>
   </si>
   <si>
-    <t>bo_manager_a3</t>
-  </si>
-  <si>
     <t>TC_13_addNewResidentialContractWithDurationMoreThanThreeMonthsAndSinglePayment</t>
   </si>
   <si>
@@ -783,21 +765,6 @@
     <t>TC_86</t>
   </si>
   <si>
-    <t>ResidentialContract</t>
-  </si>
-  <si>
-    <t>ApproveContractLesser</t>
-  </si>
-  <si>
-    <t>ApproveContractTenant</t>
-  </si>
-  <si>
-    <t>Poroperty · #3333</t>
-  </si>
-  <si>
-    <t>10123386425</t>
-  </si>
-  <si>
     <t>https://uat-ejar3.housingapps.sa/ar/public/landing</t>
   </si>
   <si>
@@ -835,6 +802,51 @@
   </si>
   <si>
     <t>Login Module</t>
+  </si>
+  <si>
+    <t>Module 2</t>
+  </si>
+  <si>
+    <t>Create Residential Contract</t>
+  </si>
+  <si>
+    <t>Create new Residential Contract</t>
+  </si>
+  <si>
+    <t>Create new Residential Contract more than 3 months</t>
+  </si>
+  <si>
+    <t>addNewResidentialContractWithDurationMoreThanThreeMonths</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>AddResidentialContract~TC_01</t>
+  </si>
+  <si>
+    <t>1056996794</t>
+  </si>
+  <si>
+    <t>13960701</t>
+  </si>
+  <si>
+    <t>1104100571</t>
+  </si>
+  <si>
+    <t>Automation test 1</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1133,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1202,6 +1214,12 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1217,7 +1235,59 @@
     <cellStyle name="Hyperlink 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1608,12 +1678,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G5" sqref="G5"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,10 +1692,10 @@
     <col min="2" max="2" width="32.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" style="3" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -1676,10 +1746,10 @@
         <v>45</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>268</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="15" t="s">
@@ -1708,54 +1778,108 @@
         <v>1</v>
       </c>
       <c r="B3" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="32">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.2" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="B4" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="C4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A5" s="17">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="G3" s="31" t="s">
+      <c r="D5" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="H3" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="45" t="s">
+      <c r="E5" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="32">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="K5" s="46">
+        <v>1</v>
+      </c>
+      <c r="L5" s="46">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1895,10 +2019,84 @@
   <autoFilter ref="A1:L62" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="E2 E1:F1">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="12"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>$J$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>$J$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 J5" xr:uid="{5653054A-31BE-44E7-A7E2-3C79ECC9C177}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{4F439F5D-0D42-4C5F-90CE-133C74221A1B}">
+            <xm:f>NOT(ISERROR(SEARCH($J$5,J3)))</xm:f>
+            <xm:f>$J$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{D14DFE6D-1B3F-460D-ABF7-FA4D4EC25BFB}">
+            <xm:f>NOT(ISERROR(SEARCH($J$3,J3)))</xm:f>
+            <xm:f>$J$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{CEE099F7-A1B1-49B8-9AA9-B70C9AFE107D}">
+            <xm:f>NOT(ISERROR(SEARCH($J$5,J5)))</xm:f>
+            <xm:f>$J$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{174F13A1-967E-4057-8809-91E6D6207843}">
+            <xm:f>NOT(ISERROR(SEARCH($J$3,J5)))</xm:f>
+            <xm:f>$J$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J5</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1907,7 +2105,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1934,13 +2132,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>32</v>
@@ -1948,10 +2146,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -1960,10 +2158,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -1972,10 +2170,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
@@ -2017,7 +2215,7 @@
         <v>37</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>42</v>
@@ -2166,10 +2364,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>40</v>
@@ -2204,13 +2402,13 @@
         <v>20</v>
       </c>
       <c r="D6" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>149</v>
-      </c>
       <c r="F6" s="31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>24</v>
@@ -2242,16 +2440,16 @@
         <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>141</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>144</v>
       </c>
       <c r="F7" s="31" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H7" s="31" t="s">
         <v>14</v>
@@ -2312,22 +2510,22 @@
         <v>47</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
@@ -2350,22 +2548,22 @@
         <v>48</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>14</v>
@@ -2388,22 +2586,22 @@
         <v>49</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>14</v>
@@ -2426,22 +2624,22 @@
         <v>50</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>14</v>
@@ -2464,22 +2662,22 @@
         <v>51</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>14</v>
@@ -2502,22 +2700,22 @@
         <v>52</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>14</v>
@@ -2540,22 +2738,22 @@
         <v>53</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>14</v>
@@ -2578,22 +2776,22 @@
         <v>54</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>14</v>
@@ -2616,22 +2814,22 @@
         <v>55</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>14</v>
@@ -2657,19 +2855,19 @@
         <v>18</v>
       </c>
       <c r="C18" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="E18" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="26" t="s">
-        <v>113</v>
-      </c>
       <c r="F18" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>14</v>
@@ -2695,19 +2893,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="E19" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="26" t="s">
-        <v>114</v>
-      </c>
       <c r="F19" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>14</v>
@@ -2730,22 +2928,22 @@
         <v>58</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>14</v>
@@ -2768,22 +2966,22 @@
         <v>59</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>14</v>
@@ -2806,22 +3004,22 @@
         <v>60</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>14</v>
@@ -2853,13 +3051,13 @@
         <v>63</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>14</v>
@@ -2891,13 +3089,13 @@
         <v>66</v>
       </c>
       <c r="E24" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>14</v>
@@ -2929,13 +3127,13 @@
         <v>67</v>
       </c>
       <c r="E25" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>14</v>
@@ -2961,19 +3159,19 @@
         <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>14</v>
@@ -3005,13 +3203,13 @@
         <v>63</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>14</v>
@@ -3043,13 +3241,13 @@
         <v>66</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>14</v>
@@ -3081,13 +3279,13 @@
         <v>67</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>14</v>
@@ -3116,16 +3314,16 @@
         <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>14</v>
@@ -3157,13 +3355,13 @@
         <v>63</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>14</v>
@@ -3195,13 +3393,13 @@
         <v>66</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>14</v>
@@ -3233,13 +3431,13 @@
         <v>67</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>14</v>
@@ -3271,13 +3469,13 @@
         <v>63</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>14</v>
@@ -3309,13 +3507,13 @@
         <v>66</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>14</v>
@@ -3347,13 +3545,13 @@
         <v>67</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>14</v>
@@ -3385,13 +3583,13 @@
         <v>63</v>
       </c>
       <c r="E37" s="36" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>14</v>
@@ -3423,13 +3621,13 @@
         <v>66</v>
       </c>
       <c r="E38" s="36" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>14</v>
@@ -3461,13 +3659,13 @@
         <v>67</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>14</v>
@@ -3499,13 +3697,13 @@
         <v>63</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>14</v>
@@ -3537,13 +3735,13 @@
         <v>66</v>
       </c>
       <c r="E41" s="37" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>14</v>
@@ -3575,13 +3773,13 @@
         <v>67</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>14</v>
@@ -3600,20 +3798,20 @@
       </c>
     </row>
     <row r="43" spans="1:12" s="2" customFormat="1" ht="19.2" x14ac:dyDescent="0.45">
-      <c r="A43" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="48"/>
+      <c r="A43" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="50"/>
     </row>
     <row r="44" spans="1:12" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A44" s="17">
@@ -3629,13 +3827,13 @@
         <v>64</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>14</v>
@@ -3667,13 +3865,13 @@
         <v>66</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>14</v>
@@ -3705,13 +3903,13 @@
         <v>67</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>14</v>
@@ -3737,19 +3935,19 @@
         <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>14</v>
@@ -3781,13 +3979,13 @@
         <v>64</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>14</v>
@@ -3819,13 +4017,13 @@
         <v>66</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>14</v>
@@ -3857,13 +4055,13 @@
         <v>67</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>14</v>
@@ -3892,16 +4090,16 @@
         <v>68</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>14</v>
@@ -3933,13 +4131,13 @@
         <v>64</v>
       </c>
       <c r="E52" s="40" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>14</v>
@@ -3971,13 +4169,13 @@
         <v>66</v>
       </c>
       <c r="E53" s="40" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>14</v>
@@ -4009,13 +4207,13 @@
         <v>67</v>
       </c>
       <c r="E54" s="40" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>14</v>
@@ -4047,13 +4245,13 @@
         <v>64</v>
       </c>
       <c r="E55" s="41" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>14</v>
@@ -4085,13 +4283,13 @@
         <v>66</v>
       </c>
       <c r="E56" s="41" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>14</v>
@@ -4123,13 +4321,13 @@
         <v>67</v>
       </c>
       <c r="E57" s="41" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>14</v>
@@ -4187,25 +4385,25 @@
         <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>56</v>
@@ -4219,7 +4417,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>19</v>
@@ -4231,7 +4429,7 @@
         <v>36</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>73</v>
@@ -4239,23 +4437,23 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
@@ -4265,7 +4463,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="31"/>
@@ -4273,13 +4471,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>36</v>
@@ -4289,7 +4487,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="31"/>
@@ -4297,7 +4495,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>19</v>
@@ -4309,7 +4507,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>73</v>
@@ -4317,29 +4515,29 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>73</v>
@@ -4347,7 +4545,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="31"/>
@@ -4355,19 +4553,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>73</v>
@@ -4375,7 +4573,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="31"/>
@@ -4383,19 +4581,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>73</v>
@@ -4409,28 +4607,28 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -4454,26 +4652,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F51C3B-4B64-404C-B05B-8686AFBD9D63}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -4493,16 +4689,10 @@
         <v>70</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -4516,10 +4706,8 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -4534,11 +4722,9 @@
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -4551,167 +4737,115 @@
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>36</v>
+        <v>245</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>73</v>
+        <v>269</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>270</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>36</v>
+        <v>245</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
-      <c r="G6" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
-      <c r="G7" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>36</v>
+        <v>245</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
-      <c r="G9" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>140</v>
+        <v>267</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>36</v>
+        <v>245</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{5DBCE85C-3755-4910-BFE8-23E3BF6BBAD6}"/>
-    <hyperlink ref="B3:B10" r:id="rId2" display="https://test-ejar3.housingapps.sa/" xr:uid="{F56E4547-28EB-497A-9400-A17357448769}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4743,7 +4877,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>30</v>
@@ -4755,7 +4889,7 @@
         <v>70</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>56</v>
@@ -4817,7 +4951,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>19</v>
@@ -4829,27 +4963,27 @@
         <v>36</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>73</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>36</v>
@@ -4857,19 +4991,19 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
@@ -4877,13 +5011,13 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>19</v>
@@ -4895,117 +5029,117 @@
         <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>73</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J34" t="s">
         <v>28</v>
@@ -5013,7 +5147,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J35" t="s">
         <v>44</v>
@@ -5021,10 +5155,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -5032,10 +5166,10 @@
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -5043,10 +5177,10 @@
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J38" t="s">
         <v>28</v>
@@ -5057,10 +5191,10 @@
         <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J39" t="s">
         <v>44</v>
@@ -5071,10 +5205,10 @@
         <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>